<commit_message>
Update admin ,giang vien sinh vien
</commit_message>
<xml_diff>
--- a/admin/uploads/test - Copy.xlsx
+++ b/admin/uploads/test - Copy.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\BTL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\BTL\admin\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BEA77BA-4FCE-4054-BD0E-08F26EA5577C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="24240" windowHeight="12525"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,6 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -569,7 +571,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -716,6 +718,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -751,6 +770,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -926,21 +962,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H84" sqref="H84"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -957,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -974,7 +1010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -991,7 +1027,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1008,7 +1044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1025,7 +1061,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1042,7 +1078,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1059,7 +1095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1076,7 +1112,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1093,7 +1129,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1110,7 +1146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1127,7 +1163,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1144,7 +1180,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1161,7 +1197,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1178,7 +1214,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1195,7 +1231,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1212,7 +1248,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1229,7 +1265,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1246,7 +1282,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1263,7 +1299,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1280,7 +1316,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1297,7 +1333,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1314,7 +1350,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1331,7 +1367,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1348,7 +1384,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1365,7 +1401,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1382,7 +1418,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1399,7 +1435,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1416,7 +1452,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1433,7 +1469,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1450,7 +1486,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1467,7 +1503,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1484,7 +1520,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1501,7 +1537,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1518,7 +1554,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1535,7 +1571,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1552,7 +1588,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1569,7 +1605,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1586,7 +1622,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1603,7 +1639,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1620,7 +1656,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1637,7 +1673,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1654,7 +1690,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -1671,7 +1707,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1688,7 +1724,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -1705,7 +1741,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -1722,7 +1758,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1739,7 +1775,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1756,7 +1792,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1773,7 +1809,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -1790,7 +1826,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -1807,7 +1843,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -1824,7 +1860,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -1841,7 +1877,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -1858,7 +1894,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -1875,7 +1911,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -1892,7 +1928,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -1909,7 +1945,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -1926,7 +1962,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -1943,7 +1979,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -1960,7 +1996,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -1977,7 +2013,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -1994,7 +2030,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -2011,7 +2047,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -2028,7 +2064,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -2045,7 +2081,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -2062,7 +2098,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -2079,7 +2115,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -2096,7 +2132,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -2113,7 +2149,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -2130,7 +2166,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -2147,7 +2183,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -2164,7 +2200,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -2181,7 +2217,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -2198,7 +2234,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -2215,7 +2251,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -2232,7 +2268,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -2249,7 +2285,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -2266,7 +2302,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -2283,7 +2319,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -2300,7 +2336,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -2317,7 +2353,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -2334,7 +2370,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>83</v>
       </c>
@@ -2351,7 +2387,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>84</v>
       </c>
@@ -2368,7 +2404,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>85</v>
       </c>
@@ -2385,7 +2421,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>86</v>
       </c>
@@ -2402,7 +2438,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -2419,7 +2455,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>88</v>
       </c>
@@ -2436,7 +2472,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>89</v>
       </c>
@@ -2453,7 +2489,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>90</v>
       </c>
@@ -2472,96 +2508,96 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="C3" r:id="rId3"/>
-    <hyperlink ref="C4" r:id="rId4"/>
-    <hyperlink ref="C89" r:id="rId5"/>
-    <hyperlink ref="C88" r:id="rId6"/>
-    <hyperlink ref="C87" r:id="rId7"/>
-    <hyperlink ref="C86" r:id="rId8"/>
-    <hyperlink ref="C85" r:id="rId9"/>
-    <hyperlink ref="C84" r:id="rId10"/>
-    <hyperlink ref="C83" r:id="rId11"/>
-    <hyperlink ref="C82" r:id="rId12"/>
-    <hyperlink ref="C81" r:id="rId13"/>
-    <hyperlink ref="C80" r:id="rId14"/>
-    <hyperlink ref="C79" r:id="rId15"/>
-    <hyperlink ref="C78" r:id="rId16"/>
-    <hyperlink ref="C77" r:id="rId17"/>
-    <hyperlink ref="C76" r:id="rId18"/>
-    <hyperlink ref="C75" r:id="rId19"/>
-    <hyperlink ref="C74" r:id="rId20"/>
-    <hyperlink ref="C73" r:id="rId21"/>
-    <hyperlink ref="C72" r:id="rId22"/>
-    <hyperlink ref="C71" r:id="rId23"/>
-    <hyperlink ref="C70" r:id="rId24"/>
-    <hyperlink ref="C69" r:id="rId25"/>
-    <hyperlink ref="C68" r:id="rId26"/>
-    <hyperlink ref="C67" r:id="rId27"/>
-    <hyperlink ref="C66" r:id="rId28"/>
-    <hyperlink ref="C65" r:id="rId29"/>
-    <hyperlink ref="C64" r:id="rId30"/>
-    <hyperlink ref="C63" r:id="rId31"/>
-    <hyperlink ref="C62" r:id="rId32"/>
-    <hyperlink ref="C61" r:id="rId33"/>
-    <hyperlink ref="C60" r:id="rId34"/>
-    <hyperlink ref="C59" r:id="rId35"/>
-    <hyperlink ref="C58" r:id="rId36"/>
-    <hyperlink ref="C57" r:id="rId37"/>
-    <hyperlink ref="C56" r:id="rId38"/>
-    <hyperlink ref="C55" r:id="rId39"/>
-    <hyperlink ref="C54" r:id="rId40"/>
-    <hyperlink ref="C53" r:id="rId41"/>
-    <hyperlink ref="C52" r:id="rId42"/>
-    <hyperlink ref="C51" r:id="rId43"/>
-    <hyperlink ref="C5" r:id="rId44"/>
-    <hyperlink ref="C6" r:id="rId45"/>
-    <hyperlink ref="C7" r:id="rId46"/>
-    <hyperlink ref="C8" r:id="rId47"/>
-    <hyperlink ref="C9" r:id="rId48"/>
-    <hyperlink ref="C90" r:id="rId49"/>
-    <hyperlink ref="C50" r:id="rId50"/>
-    <hyperlink ref="C49" r:id="rId51"/>
-    <hyperlink ref="C48" r:id="rId52"/>
-    <hyperlink ref="C47" r:id="rId53"/>
-    <hyperlink ref="C46" r:id="rId54"/>
-    <hyperlink ref="C45" r:id="rId55"/>
-    <hyperlink ref="C44" r:id="rId56"/>
-    <hyperlink ref="C43" r:id="rId57"/>
-    <hyperlink ref="C42" r:id="rId58"/>
-    <hyperlink ref="C41" r:id="rId59"/>
-    <hyperlink ref="C40" r:id="rId60"/>
-    <hyperlink ref="C39" r:id="rId61"/>
-    <hyperlink ref="C38" r:id="rId62"/>
-    <hyperlink ref="C37" r:id="rId63"/>
-    <hyperlink ref="C36" r:id="rId64"/>
-    <hyperlink ref="C10" r:id="rId65"/>
-    <hyperlink ref="C11" r:id="rId66"/>
-    <hyperlink ref="C12" r:id="rId67"/>
-    <hyperlink ref="C13" r:id="rId68"/>
-    <hyperlink ref="C35" r:id="rId69"/>
-    <hyperlink ref="C34" r:id="rId70"/>
-    <hyperlink ref="C33" r:id="rId71"/>
-    <hyperlink ref="C32" r:id="rId72"/>
-    <hyperlink ref="C31" r:id="rId73"/>
-    <hyperlink ref="C30" r:id="rId74"/>
-    <hyperlink ref="C29" r:id="rId75"/>
-    <hyperlink ref="C28" r:id="rId76"/>
-    <hyperlink ref="C27" r:id="rId77"/>
-    <hyperlink ref="C26" r:id="rId78"/>
-    <hyperlink ref="C25" r:id="rId79"/>
-    <hyperlink ref="C24" r:id="rId80"/>
-    <hyperlink ref="C23" r:id="rId81"/>
-    <hyperlink ref="C22" r:id="rId82"/>
-    <hyperlink ref="C21" r:id="rId83"/>
-    <hyperlink ref="C20" r:id="rId84"/>
-    <hyperlink ref="C19" r:id="rId85"/>
-    <hyperlink ref="C18" r:id="rId86"/>
-    <hyperlink ref="C17" r:id="rId87"/>
-    <hyperlink ref="C16" r:id="rId88"/>
-    <hyperlink ref="C15" r:id="rId89"/>
-    <hyperlink ref="C14" r:id="rId90"/>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C89" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C88" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C87" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C86" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C85" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C84" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C83" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C82" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C81" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C80" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C79" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C78" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C77" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C76" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C75" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C74" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C73" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C72" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C71" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C70" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C69" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C68" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C67" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C66" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C65" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C64" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C63" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="C62" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="C61" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C60" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C59" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C58" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C57" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C56" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="C55" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="C54" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="C53" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="C52" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="C51" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="C5" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="C6" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="C7" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="C8" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C9" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="C90" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="C50" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="C49" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="C48" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="C47" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="C46" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="C45" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="C44" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="C43" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="C42" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="C41" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="C40" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="C39" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="C38" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="C37" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="C36" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="C10" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="C11" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="C12" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="C13" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="C35" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="C34" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="C33" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="C32" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="C31" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="C30" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="C29" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="C28" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="C27" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="C26" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="C25" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="C24" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="C23" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="C22" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="C21" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="C20" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="C19" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="C18" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="C17" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="C16" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="C15" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="C14" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId91"/>
@@ -2569,24 +2605,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>